<commit_message>
working on creating panels from MISI spreadsheet
</commit_message>
<xml_diff>
--- a/orderflex/src/App/TranslationalResearchBundle/Util/MISI_with_panels.xlsx
+++ b/orderflex/src/App/TranslationalResearchBundle/Util/MISI_with_panels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinav\Documents\WCMC\TRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC87A092-A5F3-4EB2-BEBA-FFED172E41A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D979B554-1E11-4ED1-8B09-B97B28B75780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31632" yWindow="912" windowWidth="34560" windowHeight="18552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40470" yWindow="2955" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="368">
   <si>
     <t>polyclonal</t>
   </si>
@@ -389,15 +389,9 @@
     <t>EPR6301</t>
   </si>
   <si>
-    <t>Milk Fat Globule 1 (0.2mMouse</t>
-  </si>
-  <si>
     <t>SPM291</t>
   </si>
   <si>
-    <t>Estrogen Receptor alph Rabbit</t>
-  </si>
-  <si>
     <t>EPR4097</t>
   </si>
   <si>
@@ -842,9 +836,6 @@
     <t>EGFR</t>
   </si>
   <si>
-    <t>VE-Cadherin/CD144 (0.5Mouse</t>
-  </si>
-  <si>
     <t>16B1</t>
   </si>
   <si>
@@ -893,9 +884,6 @@
     <t>FAP (1mg/mL)</t>
   </si>
   <si>
-    <t>SMA (smooth muscle acRabbit</t>
-  </si>
-  <si>
     <t>ACTA2</t>
   </si>
   <si>
@@ -1031,9 +1019,6 @@
     <t>D8I4C</t>
   </si>
   <si>
-    <t>[EPR3653]</t>
-  </si>
-  <si>
     <t>TET1</t>
   </si>
   <si>
@@ -1152,6 +1137,18 @@
   </si>
   <si>
     <t>### eof p13</t>
+  </si>
+  <si>
+    <t>Milk Fat Globule 1 (0.2m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrogen Receptor alph </t>
+  </si>
+  <si>
+    <t>VE-Cadherin/CD144 (0.5</t>
+  </si>
+  <si>
+    <t>SMA (smooth muscle ac</t>
   </si>
 </sst>
 </file>
@@ -1576,13 +1573,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
-      <selection activeCell="A463" sqref="A463"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="B342" sqref="B342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="25.36328125" customWidth="1"/>
   </cols>
@@ -1686,7 +1683,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1763,7 +1760,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1829,7 +1826,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1906,7 +1903,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1983,7 +1980,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2065,7 +2062,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2147,7 +2144,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2217,7 +2214,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2287,7 +2284,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2333,7 +2330,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2391,7 +2388,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2449,7 +2446,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2531,7 +2528,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2613,7 +2610,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2659,7 +2656,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2693,39 +2690,43 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B98" s="1"/>
+        <v>365</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C98" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2739,13 +2740,13 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>1</v>
@@ -2765,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D103" s="1"/>
     </row>
@@ -2783,19 +2784,19 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2809,19 +2810,19 @@
         <v>1</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>6</v>
@@ -2835,13 +2836,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>1</v>
@@ -2853,19 +2854,19 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2873,25 +2874,25 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D113" s="1"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>6</v>
@@ -2905,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D115" s="1"/>
     </row>
@@ -2923,19 +2924,19 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2943,13 +2944,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D119" s="1"/>
     </row>
@@ -2969,19 +2970,19 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>1</v>
@@ -2999,13 +3000,13 @@
         <v>1</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D123" s="1"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>1</v>
@@ -3017,7 +3018,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3025,19 +3026,19 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>1</v>
@@ -3049,13 +3050,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>40</v>
@@ -3087,7 +3088,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>1</v>
@@ -3099,7 +3100,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3107,13 +3108,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D133" s="1"/>
     </row>
@@ -3131,13 +3132,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>40</v>
@@ -3145,7 +3146,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>1</v>
@@ -3163,13 +3164,13 @@
         <v>1</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D137" s="1"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>1</v>
@@ -3181,7 +3182,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3189,7 +3190,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>1</v>
@@ -3201,7 +3202,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>1</v>
@@ -3213,13 +3214,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>40</v>
@@ -3227,13 +3228,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D143" s="1"/>
     </row>
@@ -3251,19 +3252,19 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D145" s="1"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3283,19 +3284,19 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D148" s="1"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>1</v>
@@ -3309,31 +3310,31 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D150" s="1"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D151" s="1"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>1</v>
@@ -3345,7 +3346,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3365,7 +3366,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>1</v>
@@ -3383,7 +3384,7 @@
         <v>1</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>6</v>
@@ -3391,7 +3392,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>1</v>
@@ -3403,7 +3404,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>40</v>
@@ -3415,7 +3416,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>1</v>
@@ -3427,7 +3428,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3465,7 +3466,7 @@
         <v>1</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>40</v>
@@ -3473,7 +3474,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>1</v>
@@ -3485,7 +3486,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>1</v>
@@ -3497,7 +3498,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>1</v>
@@ -3509,7 +3510,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3517,37 +3518,37 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D168" s="1"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D169" s="1"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>6</v>
@@ -3555,13 +3556,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D171" s="1"/>
     </row>
@@ -3579,19 +3580,19 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D173" s="1"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3599,13 +3600,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="D175" s="1"/>
     </row>
@@ -3623,13 +3624,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>6</v>
@@ -3637,13 +3638,13 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B178" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C178" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="D178" s="1"/>
     </row>
@@ -3655,13 +3656,13 @@
         <v>1</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D179" s="1"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>1</v>
@@ -3673,7 +3674,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3681,13 +3682,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D182" s="1"/>
     </row>
@@ -3705,13 +3706,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>40</v>
@@ -3719,7 +3720,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>1</v>
@@ -3737,13 +3738,13 @@
         <v>1</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D186" s="1"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>1</v>
@@ -3755,7 +3756,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3769,19 +3770,19 @@
         <v>1</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D189" s="1"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D190" s="1"/>
     </row>
@@ -3793,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>40</v>
@@ -3801,25 +3802,25 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D192" s="1"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D193" s="1"/>
     </row>
@@ -3831,13 +3832,13 @@
         <v>1</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3857,13 +3858,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>6</v>
@@ -3871,25 +3872,25 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D198" s="1"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D199" s="1"/>
     </row>
@@ -3907,7 +3908,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -3921,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D202" s="1"/>
     </row>
@@ -3933,7 +3934,7 @@
         <v>25</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D203" s="1"/>
     </row>
@@ -3945,7 +3946,7 @@
         <v>25</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>6</v>
@@ -3989,7 +3990,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -4003,7 +4004,7 @@
         <v>25</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D209" s="1"/>
     </row>
@@ -4015,7 +4016,7 @@
         <v>25</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>6</v>
@@ -4023,25 +4024,25 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D211" s="1"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D212" s="1"/>
     </row>
@@ -4059,7 +4060,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -4073,13 +4074,13 @@
         <v>25</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D215" s="1"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>1</v>
@@ -4093,25 +4094,25 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D217" s="1"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D218" s="1"/>
     </row>
@@ -4129,19 +4130,19 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D220" s="1"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -4155,19 +4156,19 @@
         <v>1</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D222" s="1"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>6</v>
@@ -4175,13 +4176,13 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D224" s="1"/>
     </row>
@@ -4199,13 +4200,13 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D226" s="1"/>
     </row>
@@ -4223,7 +4224,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -4237,19 +4238,19 @@
         <v>1</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D229" s="1"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D230" s="1"/>
     </row>
@@ -4261,7 +4262,7 @@
         <v>1</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>40</v>
@@ -4269,25 +4270,25 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D232" s="1"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D233" s="1"/>
     </row>
@@ -4299,13 +4300,13 @@
         <v>1</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D234" s="1"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -4319,13 +4320,13 @@
         <v>25</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D236" s="1"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>1</v>
@@ -4337,13 +4338,13 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>6</v>
@@ -4351,13 +4352,13 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D239" s="1"/>
     </row>
@@ -4375,19 +4376,19 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D241" s="1"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -4395,37 +4396,37 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D243" s="1"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D244" s="1"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>6</v>
@@ -4433,43 +4434,43 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D246" s="1"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D247" s="1"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D248" s="1"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -4477,37 +4478,37 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D250" s="1"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D251" s="1"/>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>6</v>
@@ -4515,25 +4516,25 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D253" s="1"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D254" s="1"/>
     </row>
@@ -4545,13 +4546,13 @@
         <v>25</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D255" s="1"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
@@ -4559,19 +4560,19 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D257" s="1"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>1</v>
@@ -4585,31 +4586,31 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D259" s="1"/>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D260" s="1"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
@@ -4629,25 +4630,25 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D263" s="1"/>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>6</v>
@@ -4655,7 +4656,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>1</v>
@@ -4679,19 +4680,19 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D267" s="1"/>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
@@ -4699,37 +4700,37 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D269" s="1"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D270" s="1"/>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>6</v>
@@ -4737,43 +4738,43 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D272" s="1"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D273" s="1"/>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D274" s="1"/>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
@@ -4781,25 +4782,25 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D276" s="1"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D277" s="1"/>
     </row>
@@ -4811,7 +4812,7 @@
         <v>1</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D278" s="1" t="s">
         <v>40</v>
@@ -4819,13 +4820,13 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D279" s="1"/>
     </row>
@@ -4855,7 +4856,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A282" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B282" s="1"/>
       <c r="C282" s="1"/>
@@ -4869,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D283" s="1"/>
     </row>
@@ -4893,7 +4894,7 @@
         <v>25</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D285" s="1" t="s">
         <v>6</v>
@@ -4919,7 +4920,7 @@
         <v>25</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D287" s="1"/>
     </row>
@@ -4937,7 +4938,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
@@ -4963,7 +4964,7 @@
         <v>25</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D291" s="1"/>
     </row>
@@ -4983,13 +4984,13 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D293" s="1"/>
     </row>
@@ -5001,7 +5002,7 @@
         <v>25</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D294" s="1"/>
     </row>
@@ -5019,7 +5020,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
@@ -5027,37 +5028,37 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D297" s="1"/>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D298" s="1"/>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D299" s="1" t="s">
         <v>6</v>
@@ -5065,7 +5066,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>1</v>
@@ -5077,19 +5078,19 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D301" s="1"/>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>1</v>
@@ -5101,7 +5102,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
@@ -5115,19 +5116,19 @@
         <v>1</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D304" s="1"/>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D305" s="1"/>
     </row>
@@ -5139,7 +5140,7 @@
         <v>1</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>40</v>
@@ -5147,13 +5148,13 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A307" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D307" s="1"/>
     </row>
@@ -5165,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D308" s="1"/>
     </row>
@@ -5183,7 +5184,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A310" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
@@ -5191,19 +5192,19 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A311" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D311" s="1"/>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>1</v>
@@ -5215,13 +5216,13 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A313" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D313" s="1" t="s">
         <v>6</v>
@@ -5229,31 +5230,31 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A314" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D314" s="1"/>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A315" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D315" s="1"/>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>1</v>
@@ -5265,7 +5266,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
@@ -5273,35 +5274,37 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A318" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B318" s="1"/>
+        <v>366</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C318" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D318" s="1"/>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A319" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D319" s="1"/>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A320" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D320" s="1" t="s">
         <v>6</v>
@@ -5309,25 +5312,25 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A321" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D321" s="1"/>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D322" s="1"/>
     </row>
@@ -5339,13 +5342,13 @@
         <v>1</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D323" s="1"/>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
@@ -5353,37 +5356,37 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D325" s="1"/>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D326" s="1"/>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A327" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D327" s="1" t="s">
         <v>40</v>
@@ -5403,19 +5406,19 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A329" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D329" s="1"/>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A330" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
@@ -5429,19 +5432,19 @@
         <v>1</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D331" s="1"/>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A332" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D332" s="1"/>
     </row>
@@ -5453,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D333" s="1" t="s">
         <v>40</v>
@@ -5461,13 +5464,13 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A334" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D334" s="1"/>
     </row>
@@ -5479,7 +5482,7 @@
         <v>1</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D335" s="1"/>
     </row>
@@ -5497,7 +5500,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A337" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B337" s="1"/>
       <c r="C337" s="1"/>
@@ -5505,7 +5508,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A338" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>1</v>
@@ -5517,7 +5520,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A339" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>1</v>
@@ -5529,13 +5532,13 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A340" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D340" s="1" t="s">
         <v>6</v>
@@ -5543,7 +5546,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A341" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>1</v>
@@ -5555,20 +5558,22 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A342" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B342" s="1"/>
+        <v>367</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C342" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D342" s="1"/>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A343" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>0</v>
@@ -5577,7 +5582,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A344" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
@@ -5597,25 +5602,25 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A346" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D346" s="1"/>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A347" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D347" s="1" t="s">
         <v>6</v>
@@ -5629,7 +5634,7 @@
         <v>1</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D348" s="1"/>
     </row>
@@ -5647,19 +5652,19 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A350" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D350" s="1"/>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A351" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B351" s="1"/>
       <c r="C351" s="1"/>
@@ -5673,19 +5678,19 @@
         <v>25</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D352" s="1"/>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D353" s="1" t="s">
         <v>40</v>
@@ -5693,19 +5698,19 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D354" s="1"/>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1</v>
@@ -5717,7 +5722,7 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B356" s="3" t="s">
         <v>1</v>
@@ -5730,7 +5735,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B357" s="3"/>
       <c r="C357" s="3"/>
@@ -5739,67 +5744,69 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B358" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C358" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D358" s="6"/>
       <c r="E358" s="7"/>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D359" s="3"/>
       <c r="E359" s="4"/>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B360" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C360" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D360" s="6"/>
+        <v>178</v>
+      </c>
+      <c r="D360" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E360" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B361" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C361" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D361" s="3"/>
       <c r="E361" s="4"/>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B362" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C362" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D362" s="6"/>
       <c r="E362" s="7"/>
@@ -5819,7 +5826,7 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B364" s="3"/>
       <c r="C364" s="3"/>
@@ -5834,81 +5841,83 @@
         <v>25</v>
       </c>
       <c r="C365" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D365" s="6"/>
       <c r="E365" s="7"/>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B366" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C366" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D366" s="3"/>
       <c r="E366" s="4"/>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B367" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C367" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="D367" s="6"/>
+        <v>299</v>
+      </c>
+      <c r="D367" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E367" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B368" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C368" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D368" s="3"/>
       <c r="E368" s="4"/>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B369" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C369" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D369" s="6"/>
       <c r="E369" s="7"/>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B370" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D370" s="3"/>
       <c r="E370" s="4"/>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B371" s="3"/>
       <c r="C371" s="3"/>
@@ -5925,7 +5934,9 @@
       <c r="C372" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D372" s="6"/>
+      <c r="D372" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E372" s="7" t="s">
         <v>6</v>
       </c>
@@ -5938,40 +5949,40 @@
         <v>1</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D373" s="6"/>
       <c r="E373" s="7"/>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B374" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D374" s="6"/>
       <c r="E374" s="7"/>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="8" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B375" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D375" s="6"/>
       <c r="E375" s="7"/>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B376" s="9" t="s">
         <v>1</v>
@@ -5982,7 +5993,7 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="8" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B377" s="9"/>
       <c r="C377" s="9"/>
@@ -5991,41 +6002,42 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B378" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C378" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D378" s="3"/>
       <c r="E378" s="4"/>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B379" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C379" s="6"/>
-      <c r="D379" s="6">
+      <c r="C379" s="6">
         <v>16</v>
       </c>
       <c r="E379" s="7"/>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B380" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C380" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D380" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="D380" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E380" s="4" t="s">
         <v>6</v>
       </c>
@@ -6071,7 +6083,7 @@
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A384" s="5" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B384" s="6"/>
       <c r="C384" s="6"/>
@@ -6080,7 +6092,7 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A385" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B385" s="3" t="s">
         <v>1</v>
@@ -6091,7 +6103,7 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A386" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B386" s="6" t="s">
         <v>1</v>
@@ -6110,14 +6122,16 @@
         <v>1</v>
       </c>
       <c r="C387" s="3"/>
-      <c r="D387" s="3"/>
+      <c r="D387" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E387" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A388" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B388" s="6" t="s">
         <v>1</v>
@@ -6139,7 +6153,7 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A390" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B390" s="3" t="s">
         <v>1</v>
@@ -6149,7 +6163,7 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A391" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B391" s="3"/>
       <c r="C391" s="3"/>
@@ -6157,13 +6171,13 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B392" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C392" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D392" s="7"/>
     </row>
@@ -6175,7 +6189,7 @@
         <v>25</v>
       </c>
       <c r="C393" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D393" s="4"/>
     </row>
@@ -6195,43 +6209,43 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A395" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B395" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C395" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D395" s="4"/>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A396" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B396" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C396" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D396" s="7"/>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A397" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B397" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C397" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D397" s="4"/>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A398" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B398" s="3"/>
       <c r="C398" s="3"/>
@@ -6239,10 +6253,10 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A399" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B399" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C399" s="6" t="s">
         <v>0</v>
@@ -6251,13 +6265,13 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A400" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B400" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C400" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D400" s="4" t="s">
         <v>40</v>
@@ -6265,19 +6279,19 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B401" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C401" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D401" s="7"/>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A402" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B402" s="6"/>
       <c r="C402" s="6"/>
@@ -6285,7 +6299,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A403" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B403" s="3" t="s">
         <v>1</v>
@@ -6295,7 +6309,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A404" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B404" s="6" t="s">
         <v>1</v>
@@ -6308,7 +6322,7 @@
         <v>82</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="4" t="s">
@@ -6337,7 +6351,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A408" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B408" s="6" t="s">
         <v>1</v>
@@ -6347,7 +6361,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A409" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B409" s="6"/>
       <c r="C409" s="6"/>
@@ -6355,7 +6369,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A410" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B410" s="3" t="s">
         <v>1</v>
@@ -6365,7 +6379,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A411" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B411" s="6" t="s">
         <v>1</v>
@@ -6378,7 +6392,7 @@
         <v>82</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="4" t="s">
@@ -6397,7 +6411,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A414" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B414" s="3" t="s">
         <v>1</v>
@@ -6417,7 +6431,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A416" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B416" s="6"/>
       <c r="C416" s="6"/>
@@ -6425,37 +6439,37 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A417" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B417" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C417" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D417" s="4"/>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A418" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B418" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C418" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D418" s="7"/>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A419" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B419" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C419" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D419" s="4" t="s">
         <v>6</v>
@@ -6463,13 +6477,13 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A420" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B420" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C420" s="6" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
       <c r="D420" s="7"/>
     </row>
@@ -6487,7 +6501,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A422" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B422" s="6" t="s">
         <v>25</v>
@@ -6499,7 +6513,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A423" s="5" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B423" s="6"/>
       <c r="C423" s="6"/>
@@ -6507,25 +6521,25 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A424" s="2" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B424" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C424" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D424" s="4"/>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A425" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B425" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C425" s="6" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D425" s="7"/>
     </row>
@@ -6537,7 +6551,7 @@
         <v>1</v>
       </c>
       <c r="C426" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D426" s="4" t="s">
         <v>40</v>
@@ -6557,19 +6571,19 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A428" s="2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B428" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C428" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D428" s="4"/>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A429" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B429" s="6" t="s">
         <v>25</v>
@@ -6581,7 +6595,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A430" s="5" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B430" s="6"/>
       <c r="C430" s="6"/>
@@ -6589,13 +6603,13 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A431" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B431" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C431" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D431" s="4"/>
     </row>
@@ -6619,13 +6633,13 @@
         <v>25</v>
       </c>
       <c r="C433" s="3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D433" s="4"/>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A434" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B434" s="6" t="s">
         <v>25</v>
@@ -6639,7 +6653,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A435" s="2" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B435" s="3" t="s">
         <v>1</v>
@@ -6651,7 +6665,7 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A436" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B436" s="6" t="s">
         <v>25</v>
@@ -6663,7 +6677,7 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A437" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B437" s="6"/>
       <c r="C437" s="6"/>
@@ -6671,25 +6685,25 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A438" s="2" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B438" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C438" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D438" s="4"/>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A439" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B439" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C439" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D439" s="7" t="s">
         <v>6</v>
@@ -6697,19 +6711,19 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A440" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B440" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C440" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D440" s="4"/>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A441" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B441" s="3"/>
       <c r="C441" s="3"/>
@@ -6717,25 +6731,25 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A442" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B442" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C442" s="6" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D442" s="7"/>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A443" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B443" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C443" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D443" s="4" t="s">
         <v>6</v>
@@ -6743,19 +6757,19 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A444" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B444" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C444" s="6" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D444" s="7"/>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A445" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B445" s="6"/>
       <c r="C445" s="6"/>
@@ -6763,7 +6777,7 @@
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A446" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B446" s="3" t="s">
         <v>1</v>
@@ -6775,13 +6789,13 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A447" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B447" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C447" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D447" s="7" t="s">
         <v>6</v>
@@ -6789,19 +6803,19 @@
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A448" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B448" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C448" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D448" s="4"/>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A449" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B449" s="3"/>
       <c r="C449" s="3"/>
@@ -6815,19 +6829,19 @@
         <v>1</v>
       </c>
       <c r="C450" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D450" s="7"/>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A451" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B451" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C451" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D451" s="4"/>
     </row>
@@ -6839,7 +6853,7 @@
         <v>1</v>
       </c>
       <c r="C452" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D452" s="7" t="s">
         <v>6</v>
@@ -6847,13 +6861,13 @@
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A453" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B453" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C453" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D453" s="4"/>
     </row>
@@ -6865,7 +6879,7 @@
         <v>1</v>
       </c>
       <c r="C454" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D454" s="7"/>
     </row>
@@ -6877,13 +6891,13 @@
         <v>25</v>
       </c>
       <c r="C455" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D455" s="4"/>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A456" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B456" s="3"/>
       <c r="C456" s="3"/>
@@ -6897,31 +6911,31 @@
         <v>25</v>
       </c>
       <c r="C457" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D457" s="7"/>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A458" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B458" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C458" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D458" s="4"/>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A459" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B459" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C459" s="6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D459" s="7" t="s">
         <v>6</v>
@@ -6929,42 +6943,42 @@
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A460" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B460" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C460" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D460" s="4"/>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A461" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B461" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C461" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D461" s="7"/>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A462" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B462" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C462" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A463" s="10" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>